<commit_message>
Completed Using Excel's LEN() Function
</commit_message>
<xml_diff>
--- a/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
+++ b/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/26 - Text Based Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1537" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3E608D-C607-4ED2-8D5B-CB23EFC29079}"/>
+  <xr:revisionPtr revIDLastSave="1544" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05CDA68A-8087-4D7B-A42F-5868DA6CD6D0}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1968,13 +1968,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4062,8 +4062,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4122,8 +4122,12 @@
         <v>110</v>
       </c>
       <c r="G3" s="17" t="str">
-        <f>RIGHT(A3,2)</f>
+        <f>RIGHT(A3,LEN(A3)-6)</f>
         <v>WW</v>
+      </c>
+      <c r="H3">
+        <f>LEN(A3)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13">
@@ -4146,8 +4150,12 @@
         <v>111</v>
       </c>
       <c r="G4" s="17" t="str">
-        <f>RIGHT(A4,2)</f>
+        <f t="shared" ref="G4:G26" si="0">RIGHT(A4,LEN(A4)-6)</f>
         <v>WW</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H26" si="1">LEN(A4)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13">
@@ -4161,9 +4169,22 @@
         <v>10.89</v>
       </c>
       <c r="D5" s="37"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="E5" s="17" t="str">
+        <f t="shared" ref="E5:E26" si="2">LEFT(A5,3)</f>
+        <v>ACM</v>
+      </c>
+      <c r="F5" s="17" t="str">
+        <f t="shared" ref="F5:F26" si="3">MID(A5,4,3)</f>
+        <v>150</v>
+      </c>
+      <c r="G5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>WW</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="13">
       <c r="A6" s="22" t="s">
@@ -4176,9 +4197,22 @@
         <v>9.75</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="E6" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F6" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>321</v>
+      </c>
+      <c r="G6" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="13">
       <c r="A7" s="22" t="s">
@@ -4191,9 +4225,22 @@
         <v>9.59</v>
       </c>
       <c r="D7" s="37"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="E7" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F7" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+      <c r="G7" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="13">
       <c r="A8" s="22" t="s">
@@ -4206,9 +4253,22 @@
         <v>10.4</v>
       </c>
       <c r="D8" s="37"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="E8" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F8" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>325</v>
+      </c>
+      <c r="G8" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="13">
       <c r="A9" s="22" t="s">
@@ -4221,9 +4281,22 @@
         <v>10.56</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="E9" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F9" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>330</v>
+      </c>
+      <c r="G9" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="13">
       <c r="A10" s="22" t="s">
@@ -4236,9 +4309,22 @@
         <v>9.75</v>
       </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="E10" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F10" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="G10" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="13">
       <c r="A11" s="22" t="s">
@@ -4251,9 +4337,22 @@
         <v>9.75</v>
       </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F11" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>460</v>
+      </c>
+      <c r="G11" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>DP</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="13">
       <c r="A12" s="22" t="s">
@@ -4266,9 +4365,22 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F12" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>530</v>
+      </c>
+      <c r="G12" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OL</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="13">
       <c r="A13" s="22" t="s">
@@ -4281,9 +4393,22 @@
         <v>5.04</v>
       </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="E13" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F13" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TF</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="13">
       <c r="A14" s="22" t="s">
@@ -4296,9 +4421,22 @@
         <v>3.9</v>
       </c>
       <c r="D14" s="37"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="E14" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F14" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="G14" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OL</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="13">
       <c r="A15" s="22" t="s">
@@ -4311,9 +4449,22 @@
         <v>4.55</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="E15" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F15" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="G15" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OL</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="13">
       <c r="A16" s="22" t="s">
@@ -4326,11 +4477,24 @@
         <v>5.2</v>
       </c>
       <c r="D16" s="37"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" ht="13">
+      <c r="E16" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F16" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="G16" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>GO</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="13">
       <c r="A17" s="22" t="s">
         <v>209</v>
       </c>
@@ -4341,11 +4505,24 @@
         <v>7.31</v>
       </c>
       <c r="D17" s="37"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" ht="13">
+      <c r="E17" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>121</v>
+      </c>
+      <c r="G17" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>BF</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="13">
       <c r="A18" s="22" t="s">
         <v>210</v>
       </c>
@@ -4356,11 +4533,24 @@
         <v>6.5</v>
       </c>
       <c r="D18" s="37"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" ht="13">
+      <c r="E18" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="G18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>PS</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13">
       <c r="A19" s="22" t="s">
         <v>178</v>
       </c>
@@ -4371,11 +4561,24 @@
         <v>4.55</v>
       </c>
       <c r="D19" s="37"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="13">
+      <c r="E19" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F19" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="G19" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0995</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="13">
       <c r="A20" s="22" t="s">
         <v>211</v>
       </c>
@@ -4386,11 +4589,24 @@
         <v>14.3</v>
       </c>
       <c r="D20" s="37"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" ht="13">
+      <c r="E20" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>BVR</v>
+      </c>
+      <c r="F20" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>590</v>
+      </c>
+      <c r="G20" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>WF</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13">
       <c r="A21" s="22" t="s">
         <v>212</v>
       </c>
@@ -4401,11 +4617,24 @@
         <v>13.81</v>
       </c>
       <c r="D21" s="37"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" ht="13">
+      <c r="E21" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>BVR</v>
+      </c>
+      <c r="F21" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>690</v>
+      </c>
+      <c r="G21" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AF</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="13">
       <c r="A22" s="22" t="s">
         <v>217</v>
       </c>
@@ -4416,11 +4645,24 @@
         <v>7.31</v>
       </c>
       <c r="D22" s="37"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" ht="13">
+      <c r="E22" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRA</v>
+      </c>
+      <c r="F22" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="G22" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="13">
       <c r="A23" s="22" t="s">
         <v>218</v>
       </c>
@@ -4431,11 +4673,24 @@
         <v>7.31</v>
       </c>
       <c r="D23" s="37"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" ht="13">
+      <c r="E23" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRA</v>
+      </c>
+      <c r="F23" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="G23" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="13">
       <c r="A24" s="22" t="s">
         <v>214</v>
       </c>
@@ -4446,11 +4701,24 @@
         <v>7.31</v>
       </c>
       <c r="D24" s="37"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="13">
+      <c r="E24" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRA</v>
+      </c>
+      <c r="F24" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="G24" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="13">
       <c r="A25" s="22" t="s">
         <v>215</v>
       </c>
@@ -4461,11 +4729,24 @@
         <v>7.64</v>
       </c>
       <c r="D25" s="37"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="13">
+      <c r="E25" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRA</v>
+      </c>
+      <c r="F25" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>310</v>
+      </c>
+      <c r="G25" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13">
       <c r="A26" s="22" t="s">
         <v>216</v>
       </c>
@@ -4476,9 +4757,22 @@
         <v>6.14</v>
       </c>
       <c r="D26" s="37"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="E26" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRA</v>
+      </c>
+      <c r="F26" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>610</v>
+      </c>
+      <c r="G26" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4569,10 +4863,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4581,11 +4875,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4594,8 +4888,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4604,8 +4898,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4614,8 +4908,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4624,8 +4918,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4634,8 +4928,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4644,8 +4938,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -4654,8 +4948,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -4664,8 +4958,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -4674,8 +4968,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -4684,8 +4978,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -4694,8 +4988,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -4704,8 +4998,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -4714,8 +5008,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -4724,8 +5018,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -4734,11 +5028,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -4749,13 +5050,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Using Excel's SEARCH() Function
</commit_message>
<xml_diff>
--- a/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
+++ b/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/26 - Text Based Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1544" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05CDA68A-8087-4D7B-A42F-5868DA6CD6D0}"/>
+  <xr:revisionPtr revIDLastSave="1563" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B43CD50-7CE4-4E02-8772-B5A7F34DDBED}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1968,13 +1968,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4062,8 +4062,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4786,8 +4786,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4812,25 +4812,65 @@
       <c r="A2" t="s">
         <v>243</v>
       </c>
+      <c r="B2" t="str">
+        <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
+        <v>Patrick</v>
+      </c>
+      <c r="C2" t="str">
+        <f>RIGHT(A2,LEN(A2)-SEARCH(" ",A2))</f>
+        <v>Marleau</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>244</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B6" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
+        <v>Joe</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C6" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
+        <v>Thornton</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>245</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Brent</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>Burns</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>246</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Joe</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavelski</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>247</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>Jones</v>
       </c>
     </row>
   </sheetData>
@@ -4863,10 +4903,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4875,11 +4915,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4888,8 +4928,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4898,8 +4938,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4908,8 +4948,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4918,8 +4958,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4928,8 +4968,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4938,8 +4978,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -4948,8 +4988,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -4958,8 +4998,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -4968,8 +5008,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -4978,8 +5018,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -4988,8 +5028,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -4998,8 +5038,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5008,8 +5048,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5018,8 +5058,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5028,18 +5068,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5050,6 +5083,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Using Excel's CONCATENATE() Function
</commit_message>
<xml_diff>
--- a/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
+++ b/26 - Text Based Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/26 - Text Based Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1563" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B43CD50-7CE4-4E02-8772-B5A7F34DDBED}"/>
+  <xr:revisionPtr revIDLastSave="1565" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97749B83-6BCB-4216-8579-9F5339728E50}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1968,13 +1968,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4786,7 +4786,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -4884,8 +4884,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4903,10 +4903,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4915,11 +4915,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4928,8 +4928,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131" t="str">
+        <f>CONCATENATE(C4," ",B4)</f>
+        <v>Joe Gonzales</v>
+      </c>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4938,8 +4941,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131" t="str">
+        <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
+        <v>Gail Scote</v>
+      </c>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4948,8 +4954,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Sheryl Kane</v>
+      </c>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4958,8 +4967,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Kendrick Hapsbuch</v>
+      </c>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4968,8 +4980,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Henders</v>
+      </c>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4978,8 +4993,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Katie Atherton</v>
+      </c>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -4988,8 +5006,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Frank Bellwood</v>
+      </c>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -4998,8 +5019,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Linda Cooper</v>
+      </c>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5008,8 +5032,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Brent Cronwith</v>
+      </c>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5018,8 +5045,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Sandrae Simpson</v>
+      </c>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5028,8 +5058,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Randy Sindole</v>
+      </c>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5038,8 +5071,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Ellen Smith</v>
+      </c>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5048,8 +5084,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuome Vuanuo</v>
+      </c>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5058,8 +5097,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Tadeuz Szcznyck</v>
+      </c>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5068,11 +5110,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Tammy Wu</v>
+      </c>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5083,13 +5135,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>